<commit_message>
Added handling of BO when doing the receiving. Shipping interface has new indicator for BO. Added further logic to importation of BO. Added a new column to bo_rapport table in order to keep track of the quantity picked.
</commit_message>
<xml_diff>
--- a/data/RP_TEST.xlsx
+++ b/data/RP_TEST.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\BO RAPPORT\BO RAPPORT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\receiving_shipping_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9441230B-A3C7-4E49-AF70-B27DFDD2EB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762AA62D-11F9-457A-AEF6-89E7FEDABB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Export!$A$1:$Q$75</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -469,7 +472,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
@@ -852,11 +855,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
@@ -877,7 +880,7 @@
     <col min="17" max="17" width="8.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -979,7 +982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2369,7 +2372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2820,7 +2823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -2869,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2967,7 +2970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -3016,7 +3019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -3167,7 +3170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -3320,7 +3323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -3424,7 +3427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -3577,7 +3580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -3628,7 +3631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -3677,7 +3680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -3777,7 +3780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -3828,7 +3831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -4030,7 +4033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -4081,7 +4084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -4130,7 +4133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -4179,7 +4182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -4232,7 +4235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -4285,7 +4288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -4336,7 +4339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -4385,7 +4388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -4436,7 +4439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -4485,7 +4488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -4536,7 +4539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -4587,7 +4590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -4636,12 +4639,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>